<commit_message>
Usando ExcelJs como plugin
</commit_message>
<xml_diff>
--- a/ModeloCreatorAuthor.xlsx
+++ b/ModeloCreatorAuthor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CD7ABA-441C-4438-AADA-C998D0B71FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD289C0E-A0F8-4383-A47C-9B6CAC6AA021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8BFFE650-50D8-45D1-9439-0B8BA1F2417D}"/>
+    <workbookView xWindow="-20520" yWindow="2295" windowWidth="20640" windowHeight="11760" xr2:uid="{8BFFE650-50D8-45D1-9439-0B8BA1F2417D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="52">
   <si>
     <t>Enunciado</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>Opção D / Imagem D</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -409,6 +412,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,9 +430,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BFA463-777B-4935-B79F-E795BA6B4C27}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,86 +871,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="16" t="e" vm="1">
+      <c r="C2" s="11" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="10">
         <v>2</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="10">
         <v>4</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="10">
         <v>6</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -976,15 +985,15 @@
         <v>18</v>
       </c>
       <c r="E1" s="1"/>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1223,26 +1232,26 @@
         <v>25</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>26</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1262,15 +1271,15 @@
         <v>28</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="12"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="15"/>
     </row>
     <row r="14" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
       <c r="E14" s="2" t="s">

</xml_diff>

<commit_message>
Usando SheetJS e identificando se o arquivo que puxei é o correto
</commit_message>
<xml_diff>
--- a/ModeloCreatorAuthor.xlsx
+++ b/ModeloCreatorAuthor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20178015-7846-4BE6-8992-D859E495EEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F147546-63D4-4ED7-B104-6F36546FDE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8BFFE650-50D8-45D1-9439-0B8BA1F2417D}"/>
+    <workbookView xWindow="-19620" yWindow="3195" windowWidth="15300" windowHeight="8325" xr2:uid="{8BFFE650-50D8-45D1-9439-0B8BA1F2417D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Nova estilização do excel base
Atribuição de cores e ajustes ortográficos
</commit_message>
<xml_diff>
--- a/ModeloCreatorAuthor.xlsx
+++ b/ModeloCreatorAuthor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8834FF5E-D8DA-48BE-9F49-40081217979A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DFA72D-2305-4756-B9E3-25B7AFB3D7BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{8BFFE650-50D8-45D1-9439-0B8BA1F2417D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Enunciado</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Organize a palavra corretamente:</t>
+  </si>
+  <si>
+    <t>Traduza pineapple?</t>
   </si>
 </sst>
 </file>
@@ -186,14 +189,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -202,8 +214,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFC900"/>
+      <color rgb="FFFF5050"/>
       <color rgb="FF00579E"/>
-      <color rgb="FFFFC900"/>
       <color rgb="FF215C98"/>
     </mruColors>
   </colors>
@@ -614,15 +627,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BFA463-777B-4935-B79F-E795BA6B4C27}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.58203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.58203125" bestFit="1" customWidth="1"/>
@@ -643,25 +656,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -669,22 +682,22 @@
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="5">
         <v>2</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="5">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="5">
         <v>6</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="5">
         <v>8</v>
       </c>
     </row>
@@ -692,42 +705,48 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="20">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="D11" s="6"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="7"/>
+    </row>
+    <row r="20" spans="5:5">
+      <c r="E20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Aprimorando o plugin SheetJS usando o ExcelJS AB#34
</commit_message>
<xml_diff>
--- a/ModeloCreatorAuthor.xlsx
+++ b/ModeloCreatorAuthor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA26F3F0-B0DD-490B-B921-E5E2684BD081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5A900C-865C-4109-BACC-BBD3505CBF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8BFFE650-50D8-45D1-9439-0B8BA1F2417D}"/>
   </bookViews>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Enunciado</t>
   </si>
@@ -85,13 +96,61 @@
   </si>
   <si>
     <t>Lista de Atividades pelo Excel Creator Author</t>
+  </si>
+  <si>
+    <t>Arrasta e Solta</t>
+  </si>
+  <si>
+    <t>Como é feito o chocolate?</t>
+  </si>
+  <si>
+    <t>Cacau</t>
+  </si>
+  <si>
+    <t>Morango</t>
+  </si>
+  <si>
+    <t>Pera</t>
+  </si>
+  <si>
+    <t>Associar</t>
+  </si>
+  <si>
+    <t>Associe</t>
+  </si>
+  <si>
+    <t>opção 1 - opção 3 - opção 2 - opção 4</t>
+  </si>
+  <si>
+    <t>Carro</t>
+  </si>
+  <si>
+    <t>Maçã</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Arvore</t>
+  </si>
+  <si>
+    <t>Jogo da memória</t>
+  </si>
+  <si>
+    <t>Ache as cartas certas</t>
+  </si>
+  <si>
+    <t>2 + 2</t>
+  </si>
+  <si>
+    <t>4 + 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,14 +179,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,10 +247,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -212,7 +262,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -557,17 +607,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BFA463-777B-4935-B79F-E795BA6B4C27}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.7109375" customWidth="1"/>
     <col min="6" max="6" width="37.85546875" bestFit="1" customWidth="1"/>
@@ -586,102 +636,393 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>4</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>6</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="4">
+        <v>4</v>
+      </c>
+      <c r="G8" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Usando o Exceljs AB#27
</commit_message>
<xml_diff>
--- a/ModeloCreatorAuthor.xlsx
+++ b/ModeloCreatorAuthor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Documents\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\PI\ExcelNode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0149BB2-0D28-4256-A7A3-DD085224A4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451140FE-1699-4EF1-99CB-7B5025CC3591}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8BFFE650-50D8-45D1-9439-0B8BA1F2417D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Enunciado</t>
   </si>
@@ -85,13 +85,19 @@
   </si>
   <si>
     <t>Lista de Atividades pelo Excel Creator Author</t>
+  </si>
+  <si>
+    <t>Selecione a Imagem</t>
+  </si>
+  <si>
+    <t>Selecionar Imagem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +243,261 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1555750</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>881933</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BF12E04-1EC9-41BF-A619-90E73E956E49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5918200" y="1460500"/>
+          <a:ext cx="800100" cy="754933"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1143350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>844900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{808C240B-2080-4E33-BEC9-EA4C1EF04FB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8045450" y="1422400"/>
+          <a:ext cx="756000" cy="756000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1041400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1560278</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>870300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0583E55E-40A6-4090-B2F5-66032681B167}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10648950" y="1447800"/>
+          <a:ext cx="518878" cy="756000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1770750</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>806800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{697B1FDF-4588-48E2-9C8E-2F5E4DDF4CC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13379450" y="1384300"/>
+          <a:ext cx="799200" cy="756000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1345300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>907150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagem 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52627092-35F6-4D2D-A1A2-877AF69EAB8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15836900" y="1441450"/>
+          <a:ext cx="799200" cy="799200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -558,33 +819,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BFA463-777B-4935-B79F-E795BA6B4C27}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" customWidth="1"/>
-    <col min="6" max="6" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" customWidth="1"/>
-    <col min="8" max="8" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="31" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.75" customWidth="1"/>
+    <col min="6" max="6" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.4140625" customWidth="1"/>
+    <col min="8" max="8" width="53.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.58203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.4140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.58203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="25">
       <c r="A1" s="7" t="s">
         <v>19</v>
       </c>
@@ -595,7 +856,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="20">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -618,7 +879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="20">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -641,7 +902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="20">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -656,7 +917,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="20">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -679,7 +940,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="76" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="D11" s="2"/>
     </row>
   </sheetData>
@@ -688,5 +962,6 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>